<commit_message>
add nomor_seri ke import data gedung
</commit_message>
<xml_diff>
--- a/storage/excel_template/temp_gedung.xlsx
+++ b/storage/excel_template/temp_gedung.xlsx
@@ -22,9 +22,6 @@
     <t>BT</t>
   </si>
   <si>
-    <t>No.</t>
-  </si>
-  <si>
     <t>LS</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>RTH</t>
+  </si>
+  <si>
+    <t>No. Seri</t>
   </si>
 </sst>
 </file>
@@ -455,9 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,79 +475,79 @@
   <sheetData>
     <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>